<commit_message>
9 & 10 Aug Attendance
9 & 10 Aug Attendance
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -218,12 +218,84 @@
         </r>
       </text>
     </comment>
+    <comment ref="G10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not informed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not well</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Informed</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -658,7 +730,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -666,11 +738,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -915,10 +987,74 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>45147</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>45148</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A2:A9"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A2:A11"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:K1048576">
       <formula1>"PRESENT, ABSENT"</formula1>
     </dataValidation>

</xml_diff>